<commit_message>
Error list has been updated
</commit_message>
<xml_diff>
--- a/error_listEM.xlsx
+++ b/error_listEM.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20382"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20384"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Andzsi\Ujratervezes\Projects\Project\gps-log-book-review-general-WestCoastCooler\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Andzsi\Ujratervezes\formygithub\GPS-logbook-review\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{ED5BD5FA-240C-4048-9047-BDA7D1111434}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{056CD756-2AB7-4130-8948-1699A0CACE6C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="11790" windowHeight="7515"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="11790" windowHeight="7515" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="error_list" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="49">
   <si>
     <t>ID</t>
   </si>
@@ -37,136 +37,154 @@
     <t>Page Number</t>
   </si>
   <si>
-    <t>Technical specification
-Spectiffications</t>
-  </si>
-  <si>
-    <t>7.3.4 a 7.3-al van egy vonalban oszlop szinten, ami hiba…</t>
+    <t>7.1.1 instead of 7.1.3.</t>
+  </si>
+  <si>
+    <t>1-11…</t>
+  </si>
+  <si>
+    <t>Grammar mistake</t>
+  </si>
+  <si>
+    <t>Too many, or not enough spaces</t>
+  </si>
+  <si>
+    <t>Structure error</t>
+  </si>
+  <si>
+    <t>Structure error - colour</t>
+  </si>
+  <si>
+    <t>Missing end of sentence sign</t>
+  </si>
+  <si>
+    <t>Typo error</t>
+  </si>
+  <si>
+    <t>Colour error</t>
+  </si>
+  <si>
+    <t>Picture title</t>
+  </si>
+  <si>
+    <t>Empty "spaces" in the document</t>
+  </si>
+  <si>
+    <t>Miscount error</t>
+  </si>
+  <si>
+    <t>Page numbering error</t>
+  </si>
+  <si>
+    <t>Footer error</t>
+  </si>
+  <si>
+    <t>6.1 in 6.2</t>
+  </si>
+  <si>
+    <t>Picture looks is bad</t>
+  </si>
+  <si>
+    <t>6-10, 12-23</t>
+  </si>
+  <si>
+    <t>There is no title under the image</t>
+  </si>
+  <si>
+    <t>Some rows have one space between the chapter number and the chapter title, others have two</t>
   </si>
   <si>
     <t>1.1, 1.2, 1.3 text is dark blue
-acc to the rest of the doc, it should be light blue</t>
-  </si>
-  <si>
-    <t>requirements
-reqquiremments</t>
-  </si>
-  <si>
-    <t>5.2-ben, missing full stop after the description of red and green</t>
-  </si>
-  <si>
-    <t>5.1-ben fura négyszög, és kihagyás a sorban</t>
-  </si>
-  <si>
-    <t>green text is red
-red text is green….</t>
-  </si>
-  <si>
-    <t>GPS logbook dowload page goes to codecool page, 
-not where it should have gone</t>
-  </si>
-  <si>
-    <t>picture title: figure… :S…</t>
-  </si>
-  <si>
-    <t>no title under the image</t>
-  </si>
-  <si>
-    <t>picture title is on the left handside</t>
-  </si>
-  <si>
-    <t>almost a whole empty page, for no reason</t>
-  </si>
-  <si>
-    <t>Register an Additional Vehicles
-an additional vehicle or
+according to the rest of the document, it should be light blue</t>
+  </si>
+  <si>
+    <t>Correct: requirements
+Incorrect: reqquiremments</t>
+  </si>
+  <si>
+    <t>Correct: Technical specification
+Incorrect: Spectiffications</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GPS logbook dowload link redirects to codecool.com , 
+not to where it should have </t>
+  </si>
+  <si>
+    <t>7.3.4 starts after the same amount of indentation as 7.3, which is not how it supposed to be</t>
+  </si>
+  <si>
+    <t>5.2</t>
+  </si>
+  <si>
+    <t>Missing full stop after the description of red and green</t>
+  </si>
+  <si>
+    <t>5.1</t>
+  </si>
+  <si>
+    <t>A few unnecessary spaces amongst the characters, and a strange rectangle-like shape</t>
+  </si>
+  <si>
+    <t>Green text is red
+Red text is green….</t>
+  </si>
+  <si>
+    <t>Link directs to the wrong site</t>
+  </si>
+  <si>
+    <t>Picture title: figure…which says nothing about what we can see</t>
+  </si>
+  <si>
+    <t>Picture title is on the left handside</t>
+  </si>
+  <si>
+    <t>Almost a whole empty page, for no reason</t>
+  </si>
+  <si>
+    <t>Incorrect: Register an Additional Vehicles
+Correct: an additional vehicle OR
 additional vehicles</t>
   </si>
   <si>
-    <t>7.1.1 instead of 7.1.3.</t>
-  </si>
-  <si>
-    <t>There are five of reports
+    <t>There are five type of reports
 image shows 4 reports</t>
   </si>
   <si>
-    <t>footer… overall
+    <t>Page is numbered incorrectly
+it says: 22/21</t>
+  </si>
+  <si>
+    <t>Page is numbered incorrectly
+it says: 23/21</t>
+  </si>
+  <si>
+    <t>Page is numbered incorrectly
+it says: 24/21</t>
+  </si>
+  <si>
+    <t>Footer… overall
 1-11: 1 codecool - 1 sw, after that it is just the sw…</t>
   </si>
   <si>
-    <t>1-11…</t>
-  </si>
-  <si>
-    <t>none of the pictures are center aligned…</t>
-  </si>
-  <si>
-    <t>6,7,8,9,10,12,13,14,15,16,17,18,19,20,21,22,23</t>
-  </si>
-  <si>
-    <t>Grammar mistake</t>
-  </si>
-  <si>
-    <t>Too many, or not enough spaces</t>
-  </si>
-  <si>
-    <t>some rows has one space between the chapter number and the chapter title, others have two</t>
-  </si>
-  <si>
-    <t>Structure error</t>
-  </si>
-  <si>
-    <t>Structure error - colour</t>
-  </si>
-  <si>
-    <t>Missing end of sentence sign</t>
-  </si>
-  <si>
-    <t>Typo error</t>
-  </si>
-  <si>
-    <t>Colour error</t>
-  </si>
-  <si>
-    <t>Link direct to the wrong site</t>
-  </si>
-  <si>
-    <t>Picture title</t>
-  </si>
-  <si>
-    <t>Empty "spaces" in the document</t>
-  </si>
-  <si>
-    <t>Miscount error</t>
-  </si>
-  <si>
-    <t>Page numbering error</t>
-  </si>
-  <si>
-    <t>Footer error</t>
-  </si>
-  <si>
-    <t>6.1 in 6.2</t>
-  </si>
-  <si>
-    <t>page is numbered incorrectly
-it says: 24/21</t>
-  </si>
-  <si>
-    <t>page is numbered incorrectly
-it says: 23/21</t>
-  </si>
-  <si>
-    <t>page is numbered incorrectly
-it says: 22/21</t>
-  </si>
-  <si>
-    <t>Picture looks is bad</t>
+    <t>None of the pictures are center aligned…</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Colour codes: </t>
+  </si>
+  <si>
+    <t>Grammar(typing) mistakes</t>
+  </si>
+  <si>
+    <t>Content mistake</t>
+  </si>
+  <si>
+    <t>Structure mistake</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -321,7 +339,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="33">
+  <fills count="38">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -501,8 +519,38 @@
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC9DF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="10">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -617,6 +665,21 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="5" tint="-0.24994659260841701"/>
+      </left>
+      <right style="thin">
+        <color theme="5" tint="-0.24994659260841701"/>
+      </right>
+      <top style="thin">
+        <color theme="5" tint="-0.24994659260841701"/>
+      </top>
+      <bottom style="thin">
+        <color theme="5" tint="-0.24994659260841701"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -662,29 +725,94 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="16" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="35" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="10" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="35" borderId="10" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="36" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="37" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="37" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="37" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="37" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="37" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="36" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="37" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="37" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="37" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -733,6 +861,12 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFFFC9DF"/>
+      <color rgb="FFFFBDD8"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -1040,359 +1174,395 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E23"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:H23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C5" sqref="C5"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="2.85546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="2.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="32.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="47.7109375" customWidth="1"/>
+    <col min="3" max="3" width="50" customWidth="1"/>
     <col min="4" max="4" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="22" style="3" customWidth="1"/>
-    <col min="6" max="6" width="36.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="22" style="1" customWidth="1"/>
+    <col min="6" max="6" width="5.5703125" customWidth="1"/>
+    <col min="7" max="7" width="13.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="4" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A2" s="4">
+      <c r="G1" s="3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A2" s="6">
         <v>1</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="D2" s="8"/>
+      <c r="E2" s="10">
+        <v>1</v>
+      </c>
+      <c r="G2" s="12"/>
+      <c r="H2" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A3" s="6">
+        <v>2</v>
+      </c>
+      <c r="B3" s="23" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="24" t="s">
+        <v>23</v>
+      </c>
+      <c r="D3" s="23"/>
+      <c r="E3" s="25">
+        <v>1</v>
+      </c>
+      <c r="G3" s="19"/>
+      <c r="H3" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4" s="6">
+        <v>3</v>
+      </c>
+      <c r="B4" s="23" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="26" t="s">
+        <v>28</v>
+      </c>
+      <c r="D4" s="23"/>
+      <c r="E4" s="25">
+        <v>1</v>
+      </c>
+      <c r="G4" s="22"/>
+      <c r="H4" s="2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" s="2" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A5" s="6">
+        <v>4</v>
+      </c>
+      <c r="B5" s="23" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" s="24" t="s">
         <v>24</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="D5" s="23"/>
+      <c r="E5" s="25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6" s="6">
         <v>5</v>
       </c>
-      <c r="E2" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A3" s="4">
-        <v>2</v>
-      </c>
-      <c r="B3" s="5" t="s">
+      <c r="B6" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="C3" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="E3" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="4">
-        <v>3</v>
-      </c>
-      <c r="B4" s="5" t="s">
+      <c r="D6" s="8"/>
+      <c r="E6" s="10">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A7" s="6">
+        <v>6</v>
+      </c>
+      <c r="B7" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="D7" s="14" t="s">
+        <v>29</v>
+      </c>
+      <c r="E7" s="10">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A8" s="6">
+        <v>7</v>
+      </c>
+      <c r="B8" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="D8" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="E8" s="10">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A9" s="6">
+        <v>8</v>
+      </c>
+      <c r="B9" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="C9" s="16" t="s">
+        <v>33</v>
+      </c>
+      <c r="D9" s="17"/>
+      <c r="E9" s="18">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A10" s="6">
+        <v>9</v>
+      </c>
+      <c r="B10" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="C10" s="16" t="s">
         <v>27</v>
       </c>
-      <c r="C4" s="7" t="s">
+      <c r="D10" s="17"/>
+      <c r="E10" s="18">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A11" s="7">
+        <v>10</v>
+      </c>
+      <c r="B11" s="27" t="s">
+        <v>14</v>
+      </c>
+      <c r="C11" s="28" t="s">
+        <v>35</v>
+      </c>
+      <c r="D11" s="29"/>
+      <c r="E11" s="30">
         <v>6</v>
       </c>
-      <c r="E4" s="4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="4">
-        <v>4</v>
-      </c>
-      <c r="B5" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="C5" s="7" t="s">
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="7">
+        <v>11</v>
+      </c>
+      <c r="B12" s="27" t="s">
+        <v>14</v>
+      </c>
+      <c r="C12" s="27" t="s">
+        <v>22</v>
+      </c>
+      <c r="D12" s="27"/>
+      <c r="E12" s="30">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" s="7">
+        <v>12</v>
+      </c>
+      <c r="B13" s="31" t="s">
+        <v>14</v>
+      </c>
+      <c r="C13" s="31" t="s">
+        <v>36</v>
+      </c>
+      <c r="D13" s="31" t="s">
+        <v>19</v>
+      </c>
+      <c r="E13" s="32">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" s="7">
+        <v>13</v>
+      </c>
+      <c r="B14" s="31" t="s">
+        <v>15</v>
+      </c>
+      <c r="C14" s="31" t="s">
+        <v>37</v>
+      </c>
+      <c r="D14" s="31"/>
+      <c r="E14" s="32">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" s="2" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A15" s="6">
+        <v>14</v>
+      </c>
+      <c r="B15" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="E5" s="4">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A6" s="4">
+      <c r="C15" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="D15" s="11"/>
+      <c r="E15" s="10">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" s="7">
+        <v>15</v>
+      </c>
+      <c r="B16" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="C16" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="5" t="s">
+      <c r="D16" s="20"/>
+      <c r="E16" s="21">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="7">
+        <v>16</v>
+      </c>
+      <c r="B17" s="27" t="s">
+        <v>14</v>
+      </c>
+      <c r="C17" s="27" t="s">
+        <v>22</v>
+      </c>
+      <c r="D17" s="29"/>
+      <c r="E17" s="30">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A18" s="6">
+        <v>17</v>
+      </c>
+      <c r="B18" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="C18" s="16" t="s">
+        <v>39</v>
+      </c>
+      <c r="D18" s="17"/>
+      <c r="E18" s="18">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A19" s="6">
+        <v>18</v>
+      </c>
+      <c r="B19" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="C19" s="16" t="s">
+        <v>40</v>
+      </c>
+      <c r="D19" s="15"/>
+      <c r="E19" s="18">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A20" s="6">
+        <v>19</v>
+      </c>
+      <c r="B20" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="C20" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="D20" s="15"/>
+      <c r="E20" s="18">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A21" s="6">
+        <v>20</v>
+      </c>
+      <c r="B21" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="C21" s="16" t="s">
+        <v>42</v>
+      </c>
+      <c r="D21" s="15"/>
+      <c r="E21" s="18">
         <v>24</v>
       </c>
-      <c r="C6" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="E6" s="4">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A7" s="4">
+    </row>
+    <row r="22" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A22" s="7">
+        <v>21</v>
+      </c>
+      <c r="B22" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="C22" s="16" t="s">
+        <v>43</v>
+      </c>
+      <c r="D22" s="15"/>
+      <c r="E22" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="C7" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="E7" s="4">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="3">
-        <v>7</v>
-      </c>
-      <c r="B8" t="s">
-        <v>30</v>
-      </c>
-      <c r="C8" t="s">
-        <v>10</v>
-      </c>
-      <c r="E8" s="3">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A9" s="4">
-        <v>8</v>
-      </c>
-      <c r="B9" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="C9" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="D9" s="8"/>
-      <c r="E9" s="4">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A10" s="4">
-        <v>9</v>
-      </c>
-      <c r="B10" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="C10" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="D10" s="8"/>
-      <c r="E10" s="4">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="3">
-        <v>10</v>
-      </c>
-      <c r="B11" t="s">
-        <v>33</v>
-      </c>
-      <c r="C11" t="s">
-        <v>13</v>
-      </c>
-      <c r="D11" s="1"/>
-      <c r="E11" s="3">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="3">
-        <v>11</v>
-      </c>
-      <c r="B12" t="s">
-        <v>33</v>
-      </c>
-      <c r="C12" t="s">
-        <v>14</v>
-      </c>
-      <c r="E12" s="3">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="3">
-        <v>12</v>
-      </c>
-      <c r="B13" t="s">
-        <v>33</v>
-      </c>
-      <c r="C13" t="s">
-        <v>15</v>
-      </c>
-      <c r="D13" t="s">
-        <v>38</v>
-      </c>
-      <c r="E13" s="3">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="3">
-        <v>13</v>
-      </c>
-      <c r="B14" t="s">
-        <v>34</v>
-      </c>
-      <c r="C14" t="s">
-        <v>16</v>
-      </c>
-      <c r="E14" s="3">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" s="5" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A15" s="4">
-        <v>14</v>
-      </c>
-      <c r="B15" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="C15" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="D15" s="8"/>
-      <c r="E15" s="4">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="3">
-        <v>15</v>
-      </c>
-      <c r="B16" t="s">
-        <v>30</v>
-      </c>
-      <c r="C16" t="s">
-        <v>18</v>
-      </c>
-      <c r="E16" s="3">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="3">
-        <v>16</v>
-      </c>
-      <c r="B17" t="s">
-        <v>33</v>
-      </c>
-      <c r="C17" t="s">
-        <v>14</v>
-      </c>
-      <c r="D17" s="1"/>
-      <c r="E17" s="3">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A18" s="4">
-        <v>17</v>
-      </c>
-      <c r="B18" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="C18" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="D18" s="8"/>
-      <c r="E18" s="4">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A19" s="4">
-        <v>18</v>
-      </c>
-      <c r="B19" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="C19" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="E19" s="4">
+    </row>
+    <row r="23" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="6">
         <v>22</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A20" s="4">
-        <v>19</v>
-      </c>
-      <c r="B20" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="C20" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="E20" s="4">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A21" s="4">
+      <c r="B23" s="23" t="s">
         <v>20</v>
       </c>
-      <c r="B21" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="C21" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="E21" s="4">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A22" s="3">
+      <c r="C23" s="23" t="s">
+        <v>44</v>
+      </c>
+      <c r="D23" s="23"/>
+      <c r="E23" s="33" t="s">
         <v>21</v>
-      </c>
-      <c r="B22" t="s">
-        <v>37</v>
-      </c>
-      <c r="C22" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="E22" s="3" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A23" s="4">
-        <v>22</v>
-      </c>
-      <c r="B23" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="C23" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="E23" s="6" t="s">
-        <v>23</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>